<commit_message>
Updated sample form with new appearances
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed choice.xlsx
+++ b/extras/sample-form/Timed choice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-choice/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E95D3A2-4813-0C40-A84E-1D680F615A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2329A3A-BABA-4144-905D-749C04BBA2B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27640" yWindow="960" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28180" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="469">
   <si>
     <t>type</t>
   </si>
@@ -2663,9 +2663,6 @@
     <t>select_one math1</t>
   </si>
   <si>
-    <t>&lt;p style="font-weight:bold;font-size:24pt;text-align:center;"&gt;3 x 4 = ?&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;span style="font-weight:bold"&gt;18&lt;/span&gt;</t>
   </si>
   <si>
@@ -2681,16 +2678,10 @@
     <t>select_multiple crops</t>
   </si>
   <si>
-    <t>Which crops do you grow?</t>
-  </si>
-  <si>
     <t>crops_grown</t>
   </si>
   <si>
     <t>crop_most</t>
-  </si>
-  <si>
-    <t>Which crop do you grow the most?</t>
   </si>
   <si>
     <t>selected(${crops_grown}, filter) or filter = -99</t>
@@ -2773,15 +2764,6 @@
 ${crop_name}</t>
   </si>
   <si>
-    <t>quick custom-timed-choice(duration=20)</t>
-  </si>
-  <si>
-    <t>custom-timed-choice(duration=15, unit='cs')</t>
-  </si>
-  <si>
-    <t>custom-timed-choice</t>
-  </si>
-  <si>
     <t>select_one colors</t>
   </si>
   <si>
@@ -2803,75 +2785,123 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>select_multiple colors</t>
-  </si>
-  <si>
     <t>sky</t>
   </si>
   <si>
-    <t>This field will not auto-advance, nor will it block input.
+    <t>custom-timed-choice(duration=10, pass=-1, advance=0)</t>
+  </si>
+  <si>
+    <t>fieldlist</t>
+  </si>
+  <si>
+    <t>Field list</t>
+  </si>
+  <si>
+    <t>fl_time</t>
+  </si>
+  <si>
+    <t>fl_labels</t>
+  </si>
+  <si>
+    <t>Complete these fields in the time allotted.</t>
+  </si>
+  <si>
+    <t>label custom-timed-choice(duration=${fl_time})</t>
+  </si>
+  <si>
+    <t>list-nolabel custom-timed-choice(duration=${fl_time}, disp=0)</t>
+  </si>
+  <si>
+    <t>Do you like your job?</t>
+  </si>
+  <si>
+    <t>Do you ever feel too much pressure at your job?</t>
+  </si>
+  <si>
+    <t>Do you make enough money at your job to live off of?</t>
+  </si>
+  <si>
+    <t>job_like</t>
+  </si>
+  <si>
+    <t>job_pressure</t>
+  </si>
+  <si>
+    <t>job_money</t>
+  </si>
+  <si>
+    <t>Timed choice</t>
+  </si>
+  <si>
+    <t>timed_choice</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>yesnotimed</t>
+  </si>
+  <si>
+    <t>select_one yesnotimed</t>
+  </si>
+  <si>
+    <t>custom-timed-choice(duration=10, pass=-1, advance=0, block=0)</t>
+  </si>
+  <si>
+    <t>custom-timed-choice(duration=15, unit='cs', continue=1)</t>
+  </si>
+  <si>
+    <t>If you exit this field, you can return with your time remaining.
+Which crops do you grow?</t>
+  </si>
+  <si>
+    <t>fl_note</t>
+  </si>
+  <si>
+    <t>This is a timed field list.</t>
+  </si>
+  <si>
+    <t>quick custom-timed-choice</t>
+  </si>
+  <si>
+    <t>custom-timed-choice(continue=1)</t>
+  </si>
+  <si>
+    <t>You can also continue with this field if you swipe back.
+Which crop do you grow the most?</t>
+  </si>
+  <si>
+    <t>This field will not auto-advance, but it will block input when your time runs out.
+Which of these colors is your favorite?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is a very basic field. No parameters are defined. It also has the "quick" appearance.&lt;/p&gt;
+&lt;br&gt;
+&lt;p style="font-weight:bold;font-size:24pt;text-align:center;"&gt;3 x 4 = ?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>This field will not auto-advance, nor will it block input. This can be helpful if an enumerator is administrating the form instead of the respondent completing it themselves.
 What color is the sky?</t>
   </si>
   <si>
-    <t>This field will not auto-advance, but it will block input.
-Which of these colors is your favorite?</t>
-  </si>
-  <si>
-    <t>custom-timed-choice(duration=10, pass=0, advance=0, block=0)</t>
-  </si>
-  <si>
-    <t>custom-timed-choice(duration=10, pass=-1, advance=0)</t>
-  </si>
-  <si>
-    <t>fieldlist</t>
-  </si>
-  <si>
-    <t>Field list</t>
-  </si>
-  <si>
-    <t>fl_time</t>
-  </si>
-  <si>
-    <t>select_one yesno</t>
-  </si>
-  <si>
-    <t>fl_labels</t>
-  </si>
-  <si>
-    <t>Complete these fields in the time allotted.</t>
-  </si>
-  <si>
-    <t>label custom-timed-choice(duration=${fl_time})</t>
-  </si>
-  <si>
-    <t>list-nolabel custom-timed-choice(duration=${fl_time}, disp=0)</t>
-  </si>
-  <si>
-    <t>Do you like your job?</t>
-  </si>
-  <si>
-    <t>Do you ever feel too much pressure at your job?</t>
-  </si>
-  <si>
-    <t>Do you make enough money at your job to live off of?</t>
-  </si>
-  <si>
-    <t>job_like</t>
-  </si>
-  <si>
-    <t>job_pressure</t>
-  </si>
-  <si>
-    <t>job_money</t>
-  </si>
-  <si>
-    <t>Timed choice</t>
-  </si>
-  <si>
-    <t>timed_choice</t>
-  </si>
-  <si>
-    <t>field-list</t>
+    <t>select_one rating</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>likert custom-timed-choice(advance=0)</t>
+  </si>
+  <si>
+    <t>minimal custom-timed-choice(advance=0, pass=-1)</t>
+  </si>
+  <si>
+    <t>This field has a likert &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance.
+How would you rate your job overall?</t>
+  </si>
+  <si>
+    <t>This is a the "minimal" &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance.
+What color is grass?</t>
   </si>
 </sst>
 </file>
@@ -5064,22 +5094,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="9" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.5" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="30.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.33203125" style="9" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
@@ -5099,7 +5129,7 @@
     <col min="25" max="16384" width="11" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5110,7 +5140,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>361</v>
@@ -5190,7 +5220,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
@@ -5334,19 +5364,19 @@
       <c r="L11" s="53"/>
       <c r="W11"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>391</v>
       </c>
       <c r="B12" t="s">
-        <v>407</v>
-      </c>
-      <c r="C12" t="s">
-        <v>392</v>
+        <v>404</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>461</v>
       </c>
       <c r="D12"/>
       <c r="G12" t="s">
-        <v>428</v>
+        <v>457</v>
       </c>
       <c r="L12" t="s">
         <v>375</v>
@@ -5360,7 +5390,7 @@
         <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C13" t="s">
         <v>358</v>
@@ -5373,7 +5403,7 @@
         <v>358</v>
       </c>
       <c r="O13" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="T13" t="s">
         <v>358</v>
@@ -5384,10 +5414,10 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C14" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D14"/>
       <c r="L14" t="s">
@@ -5406,56 +5436,56 @@
       <c r="L15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" t="s">
         <v>397</v>
       </c>
-      <c r="B16" t="s">
-        <v>399</v>
-      </c>
-      <c r="C16" t="s">
-        <v>398</v>
+      <c r="C16" s="21" t="s">
+        <v>454</v>
       </c>
       <c r="D16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G16" t="s">
-        <v>429</v>
+        <v>453</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L16" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>384</v>
       </c>
       <c r="B17" t="s">
-        <v>400</v>
-      </c>
-      <c r="C17" t="s">
-        <v>401</v>
+        <v>398</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>459</v>
       </c>
       <c r="D17" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G17" t="s">
-        <v>430</v>
+        <v>458</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="L17" t="s">
         <v>375</v>
       </c>
       <c r="T17" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -5463,10 +5493,10 @@
         <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="O18" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -5474,44 +5504,44 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="L19" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>439</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -5519,7 +5549,7 @@
         <v>139</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="O25" s="9">
         <v>15</v>
@@ -5530,77 +5560,116 @@
         <v>149</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>447</v>
+        <v>33</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="G28" s="9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>447</v>
-      </c>
       <c r="B29" s="9" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="G29" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>447</v>
-      </c>
       <c r="B30" s="9" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="B31" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>444</v>
+      <c r="B32" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -5749,11 +5818,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5777,7 +5846,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -5797,7 +5866,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5811,7 +5880,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5825,7 +5894,7 @@
         <v>377</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F4" t="s">
         <v>359</v>
@@ -5842,7 +5911,7 @@
         <v>379</v>
       </c>
       <c r="D5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F5" t="s">
         <v>378</v>
@@ -5859,7 +5928,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F6" t="s">
         <v>380</v>
@@ -5876,7 +5945,7 @@
         <v>383</v>
       </c>
       <c r="D7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F7" t="s">
         <v>382</v>
@@ -5890,10 +5959,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F8"/>
     </row>
@@ -5908,7 +5977,7 @@
         <v>386</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F9" t="s">
         <v>385</v>
@@ -5922,7 +5991,7 @@
         <v>388</v>
       </c>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D10"/>
     </row>
@@ -5934,7 +6003,7 @@
         <v>389</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D11"/>
     </row>
@@ -5946,7 +6015,7 @@
         <v>390</v>
       </c>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D12"/>
     </row>
@@ -5958,7 +6027,7 @@
         <v>360</v>
       </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D13"/>
     </row>
@@ -5973,68 +6042,167 @@
         <v>386</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B16" s="15">
         <v>2</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B17" s="15">
         <v>3</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B18" s="15">
         <v>4</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B19" s="15">
         <v>-1</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B22" s="15">
+        <v>-99</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B23" s="15">
+        <v>1</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B24" s="15">
+        <v>2</v>
+      </c>
+      <c r="C24" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B25" s="15">
+        <v>3</v>
+      </c>
+      <c r="C25" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B26" s="15">
+        <v>4</v>
+      </c>
+      <c r="C26" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B27" s="15">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B28" s="15">
+        <v>-99</v>
+      </c>
+      <c r="C28" s="15">
+        <v>-99</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:I3 A10:I2001 A8:I8 A4:C7 E4:I7">
+  <conditionalFormatting sqref="A2:I3 A8:I8 A4:C7 E4:I7 A10:I2001">
     <cfRule type="expression" dxfId="100" priority="2">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
@@ -6096,14 +6264,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006022015</v>
+        <v>2006052127</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Updated sample form with better explanations of how parameters work
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed choice.xlsx
+++ b/extras/sample-form/Timed choice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-choice/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2329A3A-BABA-4144-905D-749C04BBA2B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1CF3E1-30D5-134F-BA72-BEBC2F5E341E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28180" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26920" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="471">
   <si>
     <t>type</t>
   </si>
@@ -2851,57 +2851,91 @@
     <t>custom-timed-choice(duration=15, unit='cs', continue=1)</t>
   </si>
   <si>
-    <t>If you exit this field, you can return with your time remaining.
-Which crops do you grow?</t>
-  </si>
-  <si>
     <t>fl_note</t>
   </si>
   <si>
-    <t>This is a timed field list.</t>
-  </si>
-  <si>
     <t>quick custom-timed-choice</t>
   </si>
   <si>
     <t>custom-timed-choice(continue=1)</t>
   </si>
   <si>
-    <t>You can also continue with this field if you swipe back.
-Which crop do you grow the most?</t>
-  </si>
-  <si>
-    <t>This field will not auto-advance, but it will block input when your time runs out.
-Which of these colors is your favorite?</t>
+    <t>select_one rating</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>likert custom-timed-choice(advance=0)</t>
+  </si>
+  <si>
+    <t>minimal custom-timed-choice(advance=0, pass=-1)</t>
+  </si>
+  <si>
+    <t>intro</t>
   </si>
   <si>
     <t>&lt;p&gt;This is a very basic field. No parameters are defined. It also has the "quick" appearance.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;quick custom-timed-choice&lt;/code&gt;
 &lt;br&gt;
 &lt;p style="font-weight:bold;font-size:24pt;text-align:center;"&gt;3 x 4 = ?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>This field will not auto-advance, nor will it block input. This can be helpful if an enumerator is administrating the form instead of the respondent completing it themselves.
-What color is the sky?</t>
-  </si>
-  <si>
-    <t>select_one rating</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>likert custom-timed-choice(advance=0)</t>
-  </si>
-  <si>
-    <t>minimal custom-timed-choice(advance=0, pass=-1)</t>
-  </si>
-  <si>
-    <t>This field has a likert &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance.
-How would you rate your job overall?</t>
-  </si>
-  <si>
-    <t>This is a the "minimal" &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance.
-What color is grass?</t>
+    <t>&lt;p&gt;This is a timed field list.&lt;/p&gt;
+&lt;p&gt;Top field &lt;em&gt;appearance&lt;/em&gt;:&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;label custom-timed-choice(duration=${fl_time})&lt;/code&gt;
+&lt;p&gt;Bottom field &lt;em&gt;appearance&lt;/em&gt;:&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;list-nolabel custom-timed-choice(duration=${fl_time}, disp=0)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This sample form will demonstrate the timed-choice field plug-in. With no parameters defined, this field plug-in will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Have a timer of 10 seconds (&lt;strong&gt;duration&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Use "seconds" (s) as the display unit (&lt;strong&gt;unit&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Display the time remaining (&lt;strong&gt;disp&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Set the value of the field to -99 when time runs out if no answer had been set yet (&lt;strong&gt;pass&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Auto-advance to the next field when time runs out (&lt;strong&gt;advance&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Disallow input when time runs out (&lt;strong&gt;block&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;When they leave the field, they cannot continue with their time remaining (&lt;strong&gt;resume&lt;/strong&gt;)&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;If you would like to change these properties, define the parameters listed to the right.&lt;/p&gt;&lt;br&gt;
+&lt;p&gt;In this sample form, we will demonstrate what happens with different &lt;em&gt;appearances&lt;/em&gt; and different parameters defined. The &lt;em&gt;appearance&lt;/em&gt; of the field will be in &lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;code&lt;/code&gt; formatting.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;If you exit this field, you can return with your time remaining.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(duration=15, unit='cs', continue=1)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;Which crops do you grow?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You can also continue with this field if you swipe back.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(continue=1)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;Which crop do you grow the most?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will not auto-advance, but it will block input when your time runs out.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(duration=10, pass=-1, advance=0)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;Which of these colors is your favorite?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will not auto-advance, nor will it block input. This can be helpful if an enumerator is administrating the form instead of the respondent completing it themselves.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(duration=10, pass=-1, advance=0, block=0)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;What color is the sky?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field has a likert &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance. It will block your input after time runs out.&lt;/p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;likert custom-timed-choice(advance=0)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;How would you rate your job overall?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is a the "minimal" &lt;em&gt;appearance&lt;/em&gt;, and it will not auto-advance. It will block your input after time runs out.&lt;p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;minimal custom-timed-choice(advance=0, pass=-1)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;What color is grass?&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -3350,7 +3384,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3510,6 +3544,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -5094,18 +5129,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="9" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.5" style="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.6640625" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="30.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5364,46 +5399,42 @@
       <c r="L11" s="53"/>
       <c r="W11"/>
     </row>
-    <row r="12" spans="1:24" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:24" ht="356" x14ac:dyDescent="0.2">
+      <c r="A12" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>461</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>464</v>
+      </c>
+      <c r="D12" s="54"/>
+      <c r="G12" s="53" t="s">
+        <v>461</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="W12"/>
+    </row>
+    <row r="13" spans="1:24" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>391</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>404</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="D12"/>
-      <c r="G12" t="s">
-        <v>457</v>
-      </c>
-      <c r="L12" t="s">
-        <v>375</v>
-      </c>
-      <c r="T12" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" t="s">
-        <v>405</v>
-      </c>
-      <c r="C13" t="s">
-        <v>358</v>
+      <c r="C13" s="21" t="s">
+        <v>462</v>
       </c>
       <c r="D13"/>
       <c r="G13" t="s">
-        <v>358</v>
+        <v>455</v>
       </c>
       <c r="L13" t="s">
-        <v>358</v>
-      </c>
-      <c r="O13" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="T13" t="s">
         <v>358</v>
@@ -5411,187 +5442,197 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="s">
+        <v>405</v>
+      </c>
+      <c r="C14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14"/>
+      <c r="G14" t="s">
+        <v>358</v>
+      </c>
+      <c r="L14" t="s">
+        <v>358</v>
+      </c>
+      <c r="O14" t="s">
+        <v>406</v>
+      </c>
+      <c r="T14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>407</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>408</v>
       </c>
-      <c r="D14"/>
-      <c r="L14" t="s">
+      <c r="D15"/>
+      <c r="L15" t="s">
         <v>373</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="G15" s="53"/>
-      <c r="L15"/>
-      <c r="O15"/>
-    </row>
-    <row r="16" spans="1:24" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="G16" s="53"/>
+      <c r="L16"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>396</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>397</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" s="21" t="s">
+        <v>465</v>
+      </c>
+      <c r="D17" t="s">
         <v>422</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>453</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="I16" s="57" t="s">
+      <c r="I17" s="57" t="s">
         <v>411</v>
-      </c>
-      <c r="L16" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>384</v>
-      </c>
-      <c r="B17" t="s">
-        <v>398</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>459</v>
-      </c>
-      <c r="D17" t="s">
-        <v>423</v>
-      </c>
-      <c r="G17" t="s">
-        <v>458</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>412</v>
       </c>
       <c r="L17" t="s">
         <v>375</v>
       </c>
-      <c r="T17" t="s">
+    </row>
+    <row r="18" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>384</v>
+      </c>
+      <c r="B18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="D18" t="s">
+        <v>423</v>
+      </c>
+      <c r="G18" t="s">
+        <v>456</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="L18" t="s">
+        <v>375</v>
+      </c>
+      <c r="T18" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>139</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>400</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>402</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>403</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>424</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L20" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="68" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:20" ht="102" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>460</v>
-      </c>
-      <c r="G21" s="9" t="s">
+      <c r="C22" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:20" ht="136" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="G23" s="9" t="s">
+      <c r="C24" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O26" s="9">
         <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="119" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>451</v>
-      </c>
       <c r="B28" s="9" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>439</v>
+        <v>463</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -5599,13 +5640,13 @@
         <v>451</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -5613,63 +5654,77 @@
         <v>451</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>451</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="B34" s="9" t="s">
+    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+      <c r="C35" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>466</v>
+      <c r="C36" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -6135,7 +6190,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B23" s="15">
         <v>1</v>
@@ -6146,7 +6201,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B24" s="15">
         <v>2</v>
@@ -6157,7 +6212,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B25" s="15">
         <v>3</v>
@@ -6168,7 +6223,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B26" s="15">
         <v>4</v>
@@ -6179,7 +6234,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B27" s="15">
         <v>5</v>
@@ -6190,7 +6245,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B28" s="15">
         <v>-99</v>
@@ -6271,7 +6326,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006052127</v>
+        <v>2006161958</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Removed old parameter from sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed choice.xlsx
+++ b/extras/sample-form/Timed choice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-choice/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464739C4-BA52-9844-9FA6-B3F50DC644FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA25277-B2CC-714C-9FCD-1F639D466EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28520" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="460">
   <si>
     <t>type</t>
   </si>
@@ -2639,9 +2639,6 @@
     <t>Dates</t>
   </si>
   <si>
-    <t>select_one crops</t>
-  </si>
-  <si>
     <t>-99</t>
   </si>
   <si>
@@ -2673,18 +2670,6 @@
   </si>
   <si>
     <t>&lt;span style="font-weight:bold"&gt;0&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>select_multiple crops</t>
-  </si>
-  <si>
-    <t>crops_grown</t>
-  </si>
-  <si>
-    <t>crop_most</t>
-  </si>
-  <si>
-    <t>selected(${crops_grown}, filter) or filter = -99</t>
   </si>
   <si>
     <t>crop_name</t>
@@ -2718,15 +2703,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>not(selected(., '0') and count-selected(.) &gt; 1)</t>
-  </si>
-  <si>
-    <t>'None' must be selected by itself!</t>
-  </si>
-  <si>
-    <t>not(selected(${crops_grown}, '-99') or selected(${crops_grown}, '0'))</t>
-  </si>
-  <si>
     <t>label:عربى</t>
   </si>
   <si>
@@ -2752,12 +2728,6 @@
   </si>
   <si>
     <t>لا</t>
-  </si>
-  <si>
-    <t>ما المحاصيل التي تزرعها؟</t>
-  </si>
-  <si>
-    <t>أي محصول تزرع أكثر؟</t>
   </si>
   <si>
     <t>أنت تنمو أكثر:
@@ -2904,24 +2874,6 @@
 &lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;minimal custom-timed-choice(advance=0, pass=-1)&lt;/code&gt;
 &lt;br&gt;
 &lt;p&gt;What color is grass?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;If you exit this field, you can return with your time remaining.&lt;/p&gt;
-&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(duration=15, unit='cs', resume=1)&lt;/code&gt;
-&lt;br&gt;
-&lt;p&gt;Which crops do you grow?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>custom-timed-choice(duration=15, unit='cs', resume=1)</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;You can also resume with this field if you swipe back.&lt;/p&gt;
-&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(resume=1)&lt;/code&gt;
-&lt;br&gt;
-&lt;p&gt;Which crop do you grow the most?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>custom-timed-choice(resume=1)</t>
   </si>
   <si>
     <t>grass</t>
@@ -2943,9 +2895,7 @@
 &lt;li&gt;Display the time remaining (&lt;strong&gt;disp&lt;/strong&gt;)&lt;/li&gt;
 &lt;li&gt;Set the value of the field to -99 when time runs out if no answer had been set yet (&lt;strong&gt;pass&lt;/strong&gt;)&lt;/li&gt;
 &lt;li&gt;Auto-advance to the next field when time runs out (&lt;strong&gt;advance&lt;/strong&gt;)&lt;/li&gt;
-&lt;li&gt;Disallow input when time runs out (&lt;strong&gt;block&lt;/strong&gt;)&lt;/li&gt;
-&lt;li&gt;When they leave the field, they cannot resume with their time remaining (&lt;strong&gt;resume&lt;/strong&gt;)&lt;/li&gt;
-&lt;li&gt;Not block input when a choice is selected (&lt;strong&gt;nochange&lt;/strong&gt;)&lt;/li&gt;
+&lt;li&gt;Disallow input when time runs out (&lt;strong&gt;block&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Not block input when a choice is selected (&lt;strong&gt;nochange&lt;/strong&gt;)&lt;/li&gt;
 &lt;/ul&gt;
 &lt;p&gt;If you would like to change these properties, define the parameters listed to the right. To learn more, check out the README in the &lt;a href="https://github.com/surveycto/timed-choice" target="_blank"&gt;GitHub repository&lt;/a&gt;.&lt;/p&gt;
 &lt;br&gt;
@@ -3398,7 +3348,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3521,9 +3471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5143,10 +5090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -5189,7 +5136,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>361</v>
@@ -5413,19 +5360,19 @@
       <c r="L11" s="53"/>
       <c r="W11"/>
     </row>
-    <row r="12" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+    <row r="12" spans="1:24" ht="388" x14ac:dyDescent="0.2">
+      <c r="A12" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="57" t="s">
+        <v>449</v>
+      </c>
+      <c r="C12" s="54" t="s">
         <v>459</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>473</v>
       </c>
       <c r="D12" s="54"/>
       <c r="G12" s="53" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -5435,17 +5382,17 @@
     </row>
     <row r="13" spans="1:24" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D13"/>
       <c r="G13" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="L13" t="s">
         <v>375</v>
@@ -5459,7 +5406,7 @@
         <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C14" t="s">
         <v>358</v>
@@ -5472,7 +5419,7 @@
         <v>358</v>
       </c>
       <c r="O14" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="T14" t="s">
         <v>358</v>
@@ -5483,10 +5430,10 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C15" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D15"/>
       <c r="L15" t="s">
@@ -5505,254 +5452,202 @@
       <c r="L16"/>
       <c r="O16"/>
     </row>
-    <row r="17" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" t="s">
+        <v>395</v>
+      </c>
+      <c r="O17" t="s">
         <v>396</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>397</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>466</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
+        <v>398</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="L18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="G17" t="s">
-        <v>467</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="I17" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="L17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>384</v>
-      </c>
-      <c r="B18" t="s">
-        <v>398</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>468</v>
-      </c>
-      <c r="D18" t="s">
-        <v>423</v>
-      </c>
-      <c r="G18" t="s">
-        <v>469</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="L18" t="s">
-        <v>375</v>
-      </c>
-      <c r="T18" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C22" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="153" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B19" t="s">
-        <v>400</v>
-      </c>
-      <c r="O19" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B26" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="O26" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
-        <v>402</v>
-      </c>
-      <c r="C20" t="s">
-        <v>403</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="B28" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="L20" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="136" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>432</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="153" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="O28" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="119" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>453</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>444</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B33" s="9" t="s">
+    </row>
+    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>446</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="B35" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>458</v>
+      <c r="G36" s="9" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -5929,7 +5824,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -5949,7 +5844,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5963,7 +5858,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5977,7 +5872,7 @@
         <v>377</v>
       </c>
       <c r="D4" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F4" t="s">
         <v>359</v>
@@ -5994,7 +5889,7 @@
         <v>379</v>
       </c>
       <c r="D5" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="F5" t="s">
         <v>378</v>
@@ -6011,7 +5906,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F6" t="s">
         <v>380</v>
@@ -6028,7 +5923,7 @@
         <v>383</v>
       </c>
       <c r="D7" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F7" t="s">
         <v>382</v>
@@ -6042,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="F8"/>
     </row>
@@ -6054,138 +5949,138 @@
         <v>376</v>
       </c>
       <c r="B9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C9" t="s">
         <v>385</v>
       </c>
-      <c r="C9" t="s">
-        <v>386</v>
-      </c>
       <c r="D9" s="55" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="F9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="B10" t="s">
         <v>387</v>
       </c>
-      <c r="B10" t="s">
-        <v>388</v>
-      </c>
       <c r="C10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B13" t="s">
         <v>360</v>
       </c>
       <c r="C13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C14" t="s">
         <v>385</v>
       </c>
-      <c r="C14" t="s">
-        <v>386</v>
-      </c>
       <c r="D14" s="55" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B16" s="15">
         <v>2</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B17" s="15">
         <v>3</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B18" s="15">
         <v>4</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B19" s="15">
         <v>-1</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="B20" s="15">
         <v>1</v>
@@ -6196,7 +6091,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -6207,18 +6102,18 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="B22" s="15">
         <v>-99</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B23" s="15">
         <v>1</v>
@@ -6229,7 +6124,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B24" s="15">
         <v>2</v>
@@ -6240,7 +6135,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B25" s="15">
         <v>3</v>
@@ -6251,7 +6146,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B26" s="15">
         <v>4</v>
@@ -6262,7 +6157,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B27" s="15">
         <v>5</v>
@@ -6273,7 +6168,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="B28" s="15">
         <v>-99</v>
@@ -6347,14 +6242,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006172007</v>
+        <v>2007142119</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -6389,22 +6284,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6598,10 +6493,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="64" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="65"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -9391,10 +9286,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="66" t="s">
+      <c r="A83" s="65" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="67"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -10554,20 +10449,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="60"/>
+      <c r="B1" s="59"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="63"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10642,28 +10537,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="68"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>

<commit_message>
Removed references to removed fields
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed choice.xlsx
+++ b/extras/sample-form/Timed choice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-choice/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA25277-B2CC-714C-9FCD-1F639D466EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C1D187-7723-1F41-B068-0579E2A3CDC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28520" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="455">
   <si>
     <t>type</t>
   </si>
@@ -2672,18 +2672,6 @@
     <t>&lt;span style="font-weight:bold"&gt;0&lt;/span&gt;</t>
   </si>
   <si>
-    <t>crop_name</t>
-  </si>
-  <si>
-    <t>jr:choice-name(${crop_most}, '${crop_most}')</t>
-  </si>
-  <si>
-    <t>crop_disp</t>
-  </si>
-  <si>
-    <t>You grow the most ${crop_name}.</t>
-  </si>
-  <si>
     <t>math_so</t>
   </si>
   <si>
@@ -2728,10 +2716,6 @@
   </si>
   <si>
     <t>لا</t>
-  </si>
-  <si>
-    <t>أنت تنمو أكثر:
-${crop_name}</t>
   </si>
   <si>
     <t>select_one colors</t>
@@ -5090,7 +5074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5136,7 +5120,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>361</v>
@@ -5365,14 +5349,14 @@
         <v>33</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D12" s="54"/>
       <c r="G12" s="53" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -5385,14 +5369,14 @@
         <v>390</v>
       </c>
       <c r="B13" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D13"/>
       <c r="G13" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="L13" t="s">
         <v>375</v>
@@ -5406,7 +5390,7 @@
         <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C14" t="s">
         <v>358</v>
@@ -5419,7 +5403,7 @@
         <v>358</v>
       </c>
       <c r="O14" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="T14" t="s">
         <v>358</v>
@@ -5430,10 +5414,10 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C15" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D15"/>
       <c r="L15" t="s">
@@ -5443,211 +5427,174 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="G16" s="53"/>
-      <c r="L16"/>
-      <c r="O16"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="153" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B17" t="s">
-        <v>395</v>
-      </c>
-      <c r="O17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B23" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="O23" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
-        <v>397</v>
-      </c>
-      <c r="C18" t="s">
-        <v>398</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>414</v>
-      </c>
-      <c r="L18" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="B25" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="136" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="153" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="O26" s="9">
-        <v>15</v>
+      <c r="G26" s="9" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>149</v>
+        <v>436</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>33</v>
+        <v>436</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>451</v>
+        <v>427</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>428</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>441</v>
+        <v>151</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>436</v>
+        <v>348</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>151</v>
+        <v>410</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B36" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>448</v>
+      <c r="C33" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -5824,7 +5771,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>18</v>
@@ -5844,7 +5791,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5858,7 +5805,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5872,7 +5819,7 @@
         <v>377</v>
       </c>
       <c r="D4" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F4" t="s">
         <v>359</v>
@@ -5889,7 +5836,7 @@
         <v>379</v>
       </c>
       <c r="D5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F5" t="s">
         <v>378</v>
@@ -5906,7 +5853,7 @@
         <v>381</v>
       </c>
       <c r="D6" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F6" t="s">
         <v>380</v>
@@ -5923,7 +5870,7 @@
         <v>383</v>
       </c>
       <c r="D7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F7" t="s">
         <v>382</v>
@@ -5937,10 +5884,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F8"/>
     </row>
@@ -5955,7 +5902,7 @@
         <v>385</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F9" t="s">
         <v>384</v>
@@ -6020,56 +5967,56 @@
         <v>385</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B15" s="15">
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B16" s="15">
         <v>2</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B17" s="15">
         <v>3</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B18" s="15">
         <v>4</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B19" s="15">
         <v>-1</v>
@@ -6080,7 +6027,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B20" s="15">
         <v>1</v>
@@ -6091,7 +6038,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B21" s="15">
         <v>0</v>
@@ -6102,7 +6049,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B22" s="15">
         <v>-99</v>
@@ -6113,7 +6060,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B23" s="15">
         <v>1</v>
@@ -6124,7 +6071,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B24" s="15">
         <v>2</v>
@@ -6135,7 +6082,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B25" s="15">
         <v>3</v>
@@ -6146,7 +6093,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B26" s="15">
         <v>4</v>
@@ -6157,7 +6104,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B27" s="15">
         <v>5</v>
@@ -6168,7 +6115,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B28" s="15">
         <v>-99</v>
@@ -6242,14 +6189,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007142119</v>
+        <v>2007151358</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Updated sample form with demo of different unit
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed choice.xlsx
+++ b/extras/sample-form/Timed choice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-choice/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C1D187-7723-1F41-B068-0579E2A3CDC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587E83B-C660-7C4F-A7D3-E2D11EFF0974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28520" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="458">
   <si>
     <t>type</t>
   </si>
@@ -2884,6 +2884,18 @@
 &lt;p&gt;If you would like to change these properties, define the parameters listed to the right. To learn more, check out the README in the &lt;a href="https://github.com/surveycto/timed-choice" target="_blank"&gt;GitHub repository&lt;/a&gt;.&lt;/p&gt;
 &lt;br&gt;
 &lt;p&gt;In this sample form, we will demonstrate what happens with different &lt;em&gt;appearances&lt;/em&gt; and different parameters defined. The &lt;em&gt;appearance&lt;/em&gt; of the field will be in &lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;code&lt;/code&gt; formatting.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>diff_unit</t>
+  </si>
+  <si>
+    <t>custom-timed-choice(unit='ms', pass=-1)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field uses a different time unit, milliseconds.&lt;p&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-choice(unit='ms', pass=-1)&lt;/code&gt;
+&lt;br&gt;
+&lt;p&gt;What color is the sun?&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -5074,11 +5086,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X33"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5597,6 +5609,20 @@
         <v>443</v>
       </c>
     </row>
+    <row r="34" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6196,7 +6222,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007151358</v>
+        <v>2007151621</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>